<commit_message>
first modification to presentation draft
</commit_message>
<xml_diff>
--- a/kojak_work/Stocks Track Record.xlsx
+++ b/kojak_work/Stocks Track Record.xlsx
@@ -499,16 +499,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>